<commit_message>
Added and fixed lstm.py, bugfixes in randomforest.py
</commit_message>
<xml_diff>
--- a/data/performance/model_performance.xlsx
+++ b/data/performance/model_performance.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="arima" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rf" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rf" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="lstm" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,28 +483,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5</v>
+        <v>0.5112219451371571</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4585427135678392</v>
+        <v>0.4314214463840399</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4849246231155779</v>
+        <v>0.5037406483790524</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4974874371859296</v>
+        <v>0.456359102244389</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4874371859296482</v>
+        <v>0.4488778054862843</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4447236180904522</v>
+        <v>0.5087281795511222</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4849246231155779</v>
+        <v>0.4987531172069826</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4949748743718593</v>
+        <v>0.5561097256857855</v>
       </c>
     </row>
     <row r="3">
@@ -514,28 +514,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5144124168514412</v>
+        <v>0.6756756756756757</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4</v>
+        <v>0.4270833333333333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4873096446700508</v>
+        <v>0.4758620689655172</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4968474148802018</v>
+        <v>0.3975155279503105</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4639175257731959</v>
+        <v>0.4113924050632912</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4475347661188369</v>
+        <v>0.4338235294117647</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.525</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5571428571428572</v>
       </c>
     </row>
     <row r="4">
@@ -545,28 +545,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>412.0249410842983</v>
+        <v>78.40334261017935</v>
       </c>
       <c r="C4" t="n">
-        <v>2043.499594844531</v>
+        <v>0.3796945101752504</v>
       </c>
       <c r="D4" t="n">
-        <v>1133.318577284668</v>
+        <v>0.3615427946176608</v>
       </c>
       <c r="E4" t="n">
-        <v>17.26562595673663</v>
+        <v>0.008542353855724407</v>
       </c>
       <c r="F4" t="n">
-        <v>18259.2175099255</v>
+        <v>7.659918336857181</v>
       </c>
       <c r="G4" t="n">
-        <v>82554.68188645272</v>
+        <v>27.90679897716881</v>
       </c>
       <c r="H4" t="n">
-        <v>1336795.336377845</v>
+        <v>10741.31161794926</v>
       </c>
       <c r="I4" t="n">
-        <v>341257.9477558802</v>
+        <v>103.9136394821795</v>
       </c>
     </row>
     <row r="5">
@@ -576,28 +576,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.29839750040131</v>
+        <v>8.854566201129186</v>
       </c>
       <c r="C5" t="n">
-        <v>45.20508372787879</v>
+        <v>0.6161935655094513</v>
       </c>
       <c r="D5" t="n">
-        <v>33.66479730051361</v>
+        <v>0.6012842876856677</v>
       </c>
       <c r="E5" t="n">
-        <v>4.15519264977409</v>
+        <v>0.09242485518368102</v>
       </c>
       <c r="F5" t="n">
-        <v>135.1266720892863</v>
+        <v>2.767655747533855</v>
       </c>
       <c r="G5" t="n">
-        <v>287.3233055052317</v>
+        <v>5.282688612550318</v>
       </c>
       <c r="H5" t="n">
-        <v>1156.198657834304</v>
+        <v>103.6402991984743</v>
       </c>
       <c r="I5" t="n">
-        <v>584.1728748888297</v>
+        <v>10.1938039750713</v>
       </c>
     </row>
     <row r="6">
@@ -607,28 +607,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1066454257903246</v>
+        <v>0.03611511253830557</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4749992647234734</v>
+        <v>0.005987948643043344</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3158709623752563</v>
+        <v>0.005327286492916386</v>
       </c>
       <c r="E6" t="n">
-        <v>1.203997228553131</v>
+        <v>0.01469217224402913</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3084606698931855</v>
+        <v>0.005472580903409623</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3341526847781771</v>
+        <v>0.006323547321265265</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5125489758025989</v>
+        <v>0.02515096099664834</v>
       </c>
       <c r="I6" t="n">
-        <v>0.371331947451717</v>
+        <v>0.005214907209287058</v>
       </c>
     </row>
     <row r="7">
@@ -638,28 +638,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-3.380277600647072</v>
+        <v>-6.315005592893259</v>
       </c>
       <c r="C7" t="n">
-        <v>-41.98420875969418</v>
+        <v>-0.06613684666586563</v>
       </c>
       <c r="D7" t="n">
-        <v>12.756851034061</v>
+        <v>-0.0397700188065121</v>
       </c>
       <c r="E7" t="n">
-        <v>1.580346428711831</v>
+        <v>0.002788150497838946</v>
       </c>
       <c r="F7" t="n">
-        <v>113.9886459729122</v>
+        <v>-0.2585360032298287</v>
       </c>
       <c r="G7" t="n">
-        <v>114.910035052377</v>
+        <v>0.2576701283004221</v>
       </c>
       <c r="H7" t="n">
-        <v>-992.4637003119566</v>
+        <v>-50.62132899077168</v>
       </c>
       <c r="I7" t="n">
-        <v>-530.1074160319926</v>
+        <v>-1.573897774164294</v>
       </c>
     </row>
     <row r="8">
@@ -669,28 +669,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1682184389411786</v>
+        <v>0.3556942499929322</v>
       </c>
       <c r="C8" t="n">
-        <v>-12.04024186549524</v>
+        <v>0.9881939608847117</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.127512920552947</v>
+        <v>0.9840669136952048</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.13609095124522</v>
+        <v>0.994923496736837</v>
       </c>
       <c r="F8" t="n">
-        <v>-12.19746529236379</v>
+        <v>0.9833319965041305</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.449824693869081</v>
+        <v>0.9960396910661393</v>
       </c>
       <c r="H8" t="n">
-        <v>-71.13190161161471</v>
+        <v>0.4669624747535596</v>
       </c>
       <c r="I8" t="n">
-        <v>-13.66676480193159</v>
+        <v>0.9932064909565916</v>
       </c>
     </row>
   </sheetData>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4916666666666666</v>
+        <v>0.5447154471544715</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4708333333333333</v>
+        <v>0.5203252032520326</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5166666666666667</v>
+        <v>0.5338753387533876</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.5447154471544715</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5166666666666667</v>
+        <v>0.5203252032520326</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5041666666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.5094850948509485</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4833333333333333</v>
+        <v>0.5420054200542005</v>
       </c>
     </row>
     <row r="3">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.5352941176470588</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4137931034482759</v>
+        <v>0.5156695156695157</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6875</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2258064516129032</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3571428571428572</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.25</v>
+        <v>0.5230769230769231</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2</v>
+        <v>0.5094850948509485</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3684210526315789</v>
+        <v>0.5909090909090909</v>
       </c>
     </row>
     <row r="4">
@@ -823,28 +823,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>101.456011647818</v>
+        <v>5.697480619886242</v>
       </c>
       <c r="C4" t="n">
-        <v>2.483838372641928</v>
+        <v>3.971498249945091</v>
       </c>
       <c r="D4" t="n">
-        <v>1.681132951037972</v>
+        <v>3.00173506322719</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01098660267600265</v>
+        <v>0.03554718831105954</v>
       </c>
       <c r="F4" t="n">
-        <v>26.14566962993844</v>
+        <v>37.92529183524886</v>
       </c>
       <c r="G4" t="n">
-        <v>222.8145800020879</v>
+        <v>280.2300867827402</v>
       </c>
       <c r="H4" t="n">
-        <v>14361.24774031408</v>
+        <v>1207.817713495811</v>
       </c>
       <c r="I4" t="n">
-        <v>346.528225826323</v>
+        <v>417.9626792648701</v>
       </c>
     </row>
     <row r="5">
@@ -854,28 +854,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.07253749796038</v>
+        <v>2.386939592843992</v>
       </c>
       <c r="C5" t="n">
-        <v>1.576019788150494</v>
+        <v>1.992861824097469</v>
       </c>
       <c r="D5" t="n">
-        <v>1.29658511137448</v>
+        <v>1.732551604780415</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1048169961218249</v>
+        <v>0.1885396200034877</v>
       </c>
       <c r="F5" t="n">
-        <v>5.113283644580891</v>
+        <v>6.158351389393825</v>
       </c>
       <c r="G5" t="n">
-        <v>14.92697491128353</v>
+        <v>16.7400742765001</v>
       </c>
       <c r="H5" t="n">
-        <v>119.838423472249</v>
+        <v>34.75367194262803</v>
       </c>
       <c r="I5" t="n">
-        <v>18.61526862084786</v>
+        <v>20.44413557147551</v>
       </c>
     </row>
     <row r="6">
@@ -885,28 +885,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04775591743789822</v>
+        <v>0.01000047267455709</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01429396959790438</v>
+        <v>0.01928416841780949</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01229576216970111</v>
+        <v>0.01619349587629995</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03239400603664454</v>
+        <v>0.04942039684199519</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01029422385369244</v>
+        <v>0.01211904269064898</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01817570937481165</v>
+        <v>0.02031541258809129</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02816525272678505</v>
+        <v>0.0132353061016147</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01069789919954507</v>
+        <v>0.01120087218518798</v>
       </c>
     </row>
     <row r="7">
@@ -916,28 +916,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-8.435542708333106</v>
+        <v>0.840642003832148</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1256837953693374</v>
+        <v>-0.1717958370715301</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05986631373373712</v>
+        <v>0.08035640147966379</v>
       </c>
       <c r="E7" t="n">
-        <v>0.007267619373988348</v>
+        <v>0.03442302019744709</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.4772234727654862</v>
+        <v>0.2496377092066809</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5232204861354622</v>
+        <v>1.987327513655996</v>
       </c>
       <c r="H7" t="n">
-        <v>-56.94393436625266</v>
+        <v>4.541863897887025</v>
       </c>
       <c r="I7" t="n">
-        <v>1.6965972830043</v>
+        <v>3.662490803374831</v>
       </c>
     </row>
     <row r="8">
@@ -947,28 +947,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2.280388948920184</v>
+        <v>0.9399396280246173</v>
       </c>
       <c r="C8" t="n">
-        <v>0.916640249333694</v>
+        <v>0.8507132023758059</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9417142069726567</v>
+        <v>0.8659494192009241</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9563559183928634</v>
+        <v>0.9549018176175083</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9402955745619911</v>
+        <v>0.9101012164328519</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8918640464115554</v>
+        <v>0.9426621649701536</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1326656444381503</v>
+        <v>0.9233740577815442</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9721554667266855</v>
+        <v>0.9742583587575426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slight adjustments to rf and lstm architecture, finalized backtesting script, finalized performance script
</commit_message>
<xml_diff>
--- a/data/performance/model_performance.xlsx
+++ b/data/performance/model_performance.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="arima" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rf" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rf" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="lstm" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,42 +437,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>LC1</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>HG1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>NG1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>CT1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>NG1</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>HG1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>W1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>GC1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>S1</t>
         </is>
       </c>
     </row>
@@ -483,28 +468,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5</v>
+        <v>0.5075757575757576</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4585427135678392</v>
+        <v>0.4924242424242424</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4849246231155779</v>
+        <v>0.553030303030303</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4974874371859296</v>
+        <v>0.5568181818181818</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4874371859296482</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.4447236180904522</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.4849246231155779</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4949748743718593</v>
+        <v>0.5606060606060606</v>
       </c>
     </row>
     <row r="3">
@@ -514,183 +490,173 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5144124168514412</v>
+        <v>0.5114942528735632</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4</v>
+        <v>0.4605263157894737</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4873096446700508</v>
+        <v>0.5306122448979592</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4968474148802018</v>
+        <v>0.52</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4639175257731959</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.4475347661188369</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5576923076923077</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>MSE</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>412.0249410842983</v>
+        <v>0.664179104477612</v>
       </c>
       <c r="C4" t="n">
-        <v>2043.499594844531</v>
+        <v>0.5737704918032787</v>
       </c>
       <c r="D4" t="n">
-        <v>1133.318577284668</v>
+        <v>0.4193548387096774</v>
       </c>
       <c r="E4" t="n">
-        <v>17.26562595673663</v>
+        <v>0.4297520661157025</v>
       </c>
       <c r="F4" t="n">
-        <v>18259.2175099255</v>
-      </c>
-      <c r="G4" t="n">
-        <v>82554.68188645272</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1336795.336377845</v>
-      </c>
-      <c r="I4" t="n">
-        <v>341257.9477558802</v>
+        <v>0.453125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>RMSE</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.29839750040131</v>
+        <v>0.5779220779220779</v>
       </c>
       <c r="C5" t="n">
-        <v>45.20508372787879</v>
+        <v>0.5109489051094891</v>
       </c>
       <c r="D5" t="n">
-        <v>33.66479730051361</v>
+        <v>0.4684684684684685</v>
       </c>
       <c r="E5" t="n">
-        <v>4.15519264977409</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="F5" t="n">
-        <v>135.1266720892863</v>
-      </c>
-      <c r="G5" t="n">
-        <v>287.3233055052317</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1156.198657834304</v>
-      </c>
-      <c r="I5" t="n">
-        <v>584.1728748888297</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MAPE</t>
+          <t>MSE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1066454257903246</v>
+        <v>0.5254076749868896</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4749992647234734</v>
+        <v>12.55007395546618</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3158709623752563</v>
+        <v>78.05153474156621</v>
       </c>
       <c r="E6" t="n">
-        <v>1.203997228553131</v>
+        <v>0.001277324190306098</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3084606698931855</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.3341526847781771</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.5125489758025989</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.371331947451717</v>
+        <v>0.402443540099405</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>RMSE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-3.380277600647072</v>
+        <v>0.7248501051851269</v>
       </c>
       <c r="C7" t="n">
-        <v>-41.98420875969418</v>
+        <v>3.542608354795401</v>
       </c>
       <c r="D7" t="n">
-        <v>12.756851034061</v>
+        <v>8.834677964791146</v>
       </c>
       <c r="E7" t="n">
-        <v>1.580346428711831</v>
+        <v>0.03573967249858479</v>
       </c>
       <c r="F7" t="n">
-        <v>113.9886459729122</v>
-      </c>
-      <c r="G7" t="n">
-        <v>114.910035052377</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-992.4637003119566</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-530.1074160319926</v>
+        <v>0.6343843788267528</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>MAPE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.007004147823720235</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.007202447925705352</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.005294859391120561</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.01129046857424848</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.005835554272521877</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>MBE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.03034125796971708</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.354419403239761</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.170087696305045</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.006401634564138362</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.04998110422117834</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>R2</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.1682184389411786</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-12.04024186549524</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-2.127512920552947</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-3.13609095124522</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-12.19746529236379</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-2.449824693869081</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-71.13190161161471</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-13.66676480193159</v>
+      <c r="B10" t="n">
+        <v>0.9836693864218655</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9699651950643497</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9935833099304759</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9945255012841205</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9852898434218877</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,42 +681,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>LC1</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>HG1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>NG1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>CT1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>NG1</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>HG1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>W1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>GC1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>S1</t>
         </is>
       </c>
     </row>
@@ -761,28 +712,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4916666666666666</v>
+        <v>0.545045045045045</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4708333333333333</v>
+        <v>0.6036036036036037</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5166666666666667</v>
+        <v>0.581081081081081</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.5900900900900901</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5166666666666667</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.5041666666666667</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.4333333333333333</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4833333333333333</v>
+        <v>0.5585585585585585</v>
       </c>
     </row>
     <row r="3">
@@ -792,183 +734,173 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.5491803278688525</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4137931034482759</v>
+        <v>0.5728155339805825</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5494505494505495</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2258064516129032</v>
+        <v>0.5394736842105263</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3571428571428572</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.3684210526315789</v>
+        <v>0.5876288659793815</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>MSE</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>101.456011647818</v>
+        <v>0.5929203539823009</v>
       </c>
       <c r="C4" t="n">
-        <v>2.483838372641928</v>
+        <v>0.5728155339805825</v>
       </c>
       <c r="D4" t="n">
-        <v>1.681132951037972</v>
+        <v>0.4901960784313725</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01098660267600265</v>
+        <v>0.422680412371134</v>
       </c>
       <c r="F4" t="n">
-        <v>26.14566962993844</v>
-      </c>
-      <c r="G4" t="n">
-        <v>222.8145800020879</v>
-      </c>
-      <c r="H4" t="n">
-        <v>14361.24774031408</v>
-      </c>
-      <c r="I4" t="n">
-        <v>346.528225826323</v>
+        <v>0.4956521739130435</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>RMSE</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.07253749796038</v>
+        <v>0.5702127659574469</v>
       </c>
       <c r="C5" t="n">
-        <v>1.576019788150494</v>
+        <v>0.5728155339805825</v>
       </c>
       <c r="D5" t="n">
-        <v>1.29658511137448</v>
+        <v>0.5181347150259067</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1048169961218249</v>
+        <v>0.4739884393063584</v>
       </c>
       <c r="F5" t="n">
-        <v>5.113283644580891</v>
-      </c>
-      <c r="G5" t="n">
-        <v>14.92697491128353</v>
-      </c>
-      <c r="H5" t="n">
-        <v>119.838423472249</v>
-      </c>
-      <c r="I5" t="n">
-        <v>18.61526862084786</v>
+        <v>0.5377358490566038</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MAPE</t>
+          <t>MSE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04775591743789822</v>
+        <v>0.0001696084117883182</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01429396959790438</v>
+        <v>6.659726356856363e-05</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01229576216970111</v>
+        <v>8.101945867284967e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03239400603664454</v>
+        <v>0.0008126461726668359</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01029422385369244</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.01817570937481165</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.02816525272678505</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.01069789919954507</v>
+        <v>0.0001102823523472561</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>RMSE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-8.435542708333106</v>
+        <v>0.01302337943040585</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1256837953693374</v>
+        <v>0.008160714648152063</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05986631373373712</v>
+        <v>0.009001080972463788</v>
       </c>
       <c r="E7" t="n">
-        <v>0.007267619373988348</v>
+        <v>0.02850694955036115</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.4772234727654862</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.5232204861354622</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-56.94393436625266</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.6965972830043</v>
+        <v>0.01050154047496157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>MAPE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.002263566149160649</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.001063206839006481</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.000995847991674888</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0258673837823947</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001834263138152104</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>MBE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.001069190089413396</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.001812881680779923</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.00269103750492043</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.001367960735944202</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0004642549673558569</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>R2</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>-2.280388948920184</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.916640249333694</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.9417142069726567</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.9563559183928634</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.9402955745619911</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.8918640464115554</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.1326656444381503</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.9721554667266855</v>
+      <c r="B10" t="n">
+        <v>0.9561638873085722</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9750785278859864</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.988342410021797</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9834738319172183</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9717965806113718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>